<commit_message>
Updated README and CodeBooks
</commit_message>
<xml_diff>
--- a/Ottoman-Algeria-Constantine_Governors-Data.xlsx
+++ b/Ottoman-Algeria-Constantine_Governors-Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="26715" windowHeight="9840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26715" windowHeight="9840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ConstantineBeys" sheetId="1" r:id="rId1"/>
@@ -1505,28 +1505,6 @@
   </si>
   <si>
     <r>
-      <t>Al-ʿAntarī, Ṣāliḥ Ibn Muḥammad.</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Farīdah manīsah [sic] fī ḥāl dukhūl al-Turk balad Qusanṭīnah wa-istīlāʾihim ʻalā awṭānihimā, aw, Tāʾrīkh Qusanṭīnah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">. Edited by Yaḥyā Bū ʿAzīz. Algeria: Dīwān al-Maṭbūʿāt al-Jāmiʿiyyah, 1991.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>This information is based on identity markers that source authors used, such as "turc d'origine" (Turk by origin), "kouloughli" (</t>
     </r>
     <r>
@@ -1548,6 +1526,27 @@
   </si>
   <si>
     <t>Source node ID for the first individual</t>
+  </si>
+  <si>
+    <r>
+      <t>Al-ʿAntarī, Ṣāliḥ Ibn Muḥammad.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Farīdah manīsah [sic] fī ḥāl dukhūl al-Turk balad Qusanṭīnah wa-istīlāʾihim ʻalā awṭānihimā, aw, Tāʾrīkh Qusanṭīnah</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>. Edited by Yaḥyā Bū ʿAzīz. Algeria: Dīwān al-Maṭbūʿāt al-Jāmiʿiyyah, 1991.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1652,7 +1651,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1693,12 +1692,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDBE5F1"/>
         <bgColor rgb="FFDBE5F1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9BBB59"/>
-        <bgColor rgb="FF9BBB59"/>
       </patternFill>
     </fill>
   </fills>
@@ -1758,9 +1751,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1857,16 +1847,19 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2215,7 +2208,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2237,2940 +2230,2940 @@
     <col min="23" max="23" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="24" customFormat="1" ht="38.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:23" s="23" customFormat="1" ht="38.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="T1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="23" t="s">
+      <c r="V1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="W1" s="22" t="s">
+      <c r="W1" s="21" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="24" customFormat="1" ht="191.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:23" s="23" customFormat="1" ht="191.25">
+      <c r="A2" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27">
         <v>1567</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28">
         <v>1574</v>
       </c>
-      <c r="J2" s="29">
+      <c r="J2" s="28">
         <v>7</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N2" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P2" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q2" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R2" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T2" s="31" t="s">
+      <c r="M2" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="U2" s="31" t="s">
+      <c r="U2" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="V2" s="32" t="s">
+      <c r="V2" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="W2" s="32"/>
-    </row>
-    <row r="3" spans="1:23" s="24" customFormat="1" ht="51">
-      <c r="A3" s="25" t="s">
+      <c r="W2" s="31"/>
+    </row>
+    <row r="3" spans="1:23" s="23" customFormat="1" ht="51">
+      <c r="A3" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28">
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27">
         <v>1574</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28">
         <v>1588</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="28">
         <v>14</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="L3" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N3" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P3" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" s="30" t="s">
+      <c r="M3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q3" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="R3" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S3" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T3" s="35" t="s">
+      <c r="R3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="U3" s="31" t="s">
+      <c r="U3" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="V3" s="32"/>
-      <c r="W3" s="32"/>
-    </row>
-    <row r="4" spans="1:23" s="24" customFormat="1" ht="31.5">
-      <c r="A4" s="25" t="s">
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+    </row>
+    <row r="4" spans="1:23" s="23" customFormat="1" ht="31.5">
+      <c r="A4" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28">
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27">
         <v>1588</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29">
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28">
         <v>1608</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="28">
         <v>20</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="M4" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" s="30" t="s">
+      <c r="M4" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="Q4" s="30" t="s">
+      <c r="Q4" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="R4" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S4" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T4" s="35" t="s">
+      <c r="R4" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="U4" s="31" t="s">
+      <c r="U4" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-    </row>
-    <row r="5" spans="1:23" s="24" customFormat="1" ht="26.25">
-      <c r="A5" s="32" t="s">
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+    </row>
+    <row r="5" spans="1:23" s="23" customFormat="1" ht="26.25">
+      <c r="A5" s="31" t="s">
         <v>126</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28">
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27">
         <v>1608</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29">
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28">
         <v>1622</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="28">
         <v>14</v>
       </c>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M5" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N5" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O5" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P5" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q5" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R5" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S5" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T5" s="35" t="s">
+      <c r="M5" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q5" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R5" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S5" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T5" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="U5" s="31"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="32"/>
-    </row>
-    <row r="6" spans="1:23" s="24" customFormat="1" ht="216.75">
-      <c r="A6" s="32" t="s">
+      <c r="U5" s="30"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+    </row>
+    <row r="6" spans="1:23" s="23" customFormat="1" ht="216.75">
+      <c r="A6" s="31" t="s">
         <v>130</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28">
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27">
         <v>1622</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29">
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28">
         <v>1647</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="27">
         <f>I6-F6</f>
         <v>25</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="K6" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="29" t="s">
+      <c r="L6" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="29">
         <v>1</v>
       </c>
-      <c r="N6" s="30" t="s">
+      <c r="N6" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="O6" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P6" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q6" s="30" t="s">
+      <c r="O6" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P6" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q6" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="R6" s="30">
+      <c r="R6" s="29">
         <v>0</v>
       </c>
-      <c r="S6" s="30" t="s">
+      <c r="S6" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="T6" s="37" t="s">
+      <c r="T6" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="U6" s="38" t="s">
+      <c r="U6" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="V6" s="32" t="s">
+      <c r="V6" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="W6" s="32" t="s">
+      <c r="W6" s="31" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="24" customFormat="1" ht="128.25">
-      <c r="A7" s="32" t="s">
+    <row r="7" spans="1:23" s="23" customFormat="1" ht="128.25">
+      <c r="A7" s="31" t="s">
         <v>138</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28">
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27">
         <v>1647</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="29">
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28">
         <v>1653</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="28">
         <v>6</v>
       </c>
-      <c r="K7" s="30" t="s">
+      <c r="K7" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="L7" s="30" t="s">
+      <c r="L7" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="M7" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O7" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P7" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q7" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R7" s="30">
+      <c r="M7" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O7" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P7" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q7" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R7" s="29">
         <v>0</v>
       </c>
-      <c r="S7" s="30" t="s">
+      <c r="S7" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="T7" s="37" t="s">
+      <c r="T7" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="U7" s="38" t="s">
+      <c r="U7" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="V7" s="32" t="s">
+      <c r="V7" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="W7" s="30"/>
-    </row>
-    <row r="8" spans="1:23" s="24" customFormat="1" ht="64.5">
-      <c r="A8" s="32" t="s">
+      <c r="W7" s="29"/>
+    </row>
+    <row r="8" spans="1:23" s="23" customFormat="1" ht="64.5">
+      <c r="A8" s="31" t="s">
         <v>144</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28">
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27">
         <v>1653</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="29">
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28">
         <v>1666</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="28">
         <v>13</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="K8" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="M8" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N8" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O8" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P8" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q8" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R8" s="30">
+      <c r="M8" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P8" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q8" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R8" s="29">
         <v>1</v>
       </c>
-      <c r="S8" s="30" t="s">
+      <c r="S8" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="T8" s="37" t="s">
+      <c r="T8" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="U8" s="38" t="s">
+      <c r="U8" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="V8" s="30" t="s">
+      <c r="V8" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="W8" s="30"/>
-    </row>
-    <row r="9" spans="1:23" s="24" customFormat="1" ht="89.25">
-      <c r="A9" s="32" t="s">
+      <c r="W8" s="29"/>
+    </row>
+    <row r="9" spans="1:23" s="23" customFormat="1" ht="89.25">
+      <c r="A9" s="31" t="s">
         <v>150</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="27">
         <v>10</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28">
+      <c r="E9" s="27"/>
+      <c r="F9" s="27">
         <v>1666</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="29">
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28">
         <v>1672</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="28">
         <v>6</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="M9" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N9" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O9" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P9" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q9" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R9" s="30">
+      <c r="M9" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O9" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P9" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q9" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R9" s="29">
         <v>1</v>
       </c>
-      <c r="S9" s="30" t="s">
+      <c r="S9" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="T9" s="37" t="s">
+      <c r="T9" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="U9" s="39" t="s">
+      <c r="U9" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="V9" s="32" t="s">
+      <c r="V9" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="W9" s="30" t="s">
+      <c r="W9" s="29" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="24" customFormat="1" ht="360.75">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:23" s="23" customFormat="1" ht="360.75">
+      <c r="A10" s="31" t="s">
         <v>158</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28">
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27">
         <v>1672</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28">
+      <c r="G10" s="27"/>
+      <c r="H10" s="27">
         <v>4</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="28">
         <v>1676</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="28">
         <v>3</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="K10" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="L10" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="M10" s="30">
+      <c r="L10" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10" s="29">
         <v>1</v>
       </c>
-      <c r="N10" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O10" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P10" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q10" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R10" s="30">
+      <c r="N10" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O10" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P10" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q10" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R10" s="29">
         <v>1</v>
       </c>
-      <c r="S10" s="30" t="s">
+      <c r="S10" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="T10" s="37" t="s">
+      <c r="T10" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="U10" s="31" t="s">
+      <c r="U10" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="V10" s="41" t="s">
+      <c r="V10" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="W10" s="30" t="s">
+      <c r="W10" s="29" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="24" customFormat="1" ht="102.75">
-      <c r="A11" s="32" t="s">
+    <row r="11" spans="1:23" s="23" customFormat="1" ht="102.75">
+      <c r="A11" s="31" t="s">
         <v>165</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="27">
         <v>4</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28">
+      <c r="E11" s="27"/>
+      <c r="F11" s="27">
         <v>1676</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="29">
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28">
         <v>1679</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="28">
         <v>3</v>
       </c>
-      <c r="K11" s="30" t="s">
+      <c r="K11" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L11" s="29" t="s">
+      <c r="L11" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M11" s="30">
+      <c r="M11" s="29">
         <v>1</v>
       </c>
-      <c r="N11" s="30" t="s">
+      <c r="N11" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="O11" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P11" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q11" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R11" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S11" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T11" s="37" t="s">
+      <c r="O11" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P11" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q11" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R11" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S11" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T11" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="U11" s="38" t="s">
+      <c r="U11" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="V11" s="42"/>
-      <c r="W11" s="30" t="s">
+      <c r="V11" s="41"/>
+      <c r="W11" s="29" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="24" customFormat="1" ht="128.25">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:23" s="23" customFormat="1" ht="128.25">
+      <c r="A12" s="31" t="s">
         <v>171</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28">
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27">
         <v>1679</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="27">
         <v>8</v>
       </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="29">
+      <c r="H12" s="27"/>
+      <c r="I12" s="28">
         <v>1688</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="28">
         <v>9</v>
       </c>
-      <c r="K12" s="30" t="s">
+      <c r="K12" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="L12" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="M12" s="30">
+      <c r="M12" s="29">
         <v>1</v>
       </c>
-      <c r="N12" s="30" t="s">
+      <c r="N12" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="O12" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P12" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q12" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R12" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S12" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T12" s="37" t="s">
+      <c r="O12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T12" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="U12" s="38" t="s">
+      <c r="U12" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="V12" s="32" t="s">
+      <c r="V12" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="W12" s="30" t="s">
+      <c r="W12" s="29" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="24" customFormat="1" ht="115.5">
-      <c r="A13" s="32" t="s">
+    <row r="13" spans="1:23" s="23" customFormat="1" ht="115.5">
+      <c r="A13" s="31" t="s">
         <v>179</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="27">
         <v>8</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28">
+      <c r="E13" s="27"/>
+      <c r="F13" s="27">
         <v>1688</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="29">
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28">
         <v>1692</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="28">
         <v>4</v>
       </c>
-      <c r="K13" s="30" t="s">
+      <c r="K13" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="L13" s="29" t="s">
+      <c r="L13" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M13" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N13" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O13" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P13" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q13" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R13" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S13" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T13" s="37" t="s">
+      <c r="M13" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O13" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P13" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q13" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R13" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S13" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T13" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="U13" s="38" t="s">
+      <c r="U13" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="V13" s="42"/>
-      <c r="W13" s="30" t="s">
+      <c r="V13" s="41"/>
+      <c r="W13" s="29" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="24" customFormat="1" ht="141">
-      <c r="A14" s="32" t="s">
+    <row r="14" spans="1:23" s="23" customFormat="1" ht="141">
+      <c r="A14" s="31" t="s">
         <v>185</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28">
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27">
         <v>1692</v>
       </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="29">
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="28">
         <v>1700</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="28">
         <v>8</v>
       </c>
-      <c r="K14" s="30" t="s">
+      <c r="K14" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="L14" s="29" t="s">
+      <c r="L14" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M14" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N14" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O14" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P14" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q14" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R14" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S14" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T14" s="37" t="s">
+      <c r="M14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T14" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="U14" s="38" t="s">
+      <c r="U14" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="V14" s="42"/>
-      <c r="W14" s="30"/>
-    </row>
-    <row r="15" spans="1:23" s="24" customFormat="1" ht="128.25">
-      <c r="A15" s="32" t="s">
+      <c r="V14" s="41"/>
+      <c r="W14" s="29"/>
+    </row>
+    <row r="15" spans="1:23" s="23" customFormat="1" ht="128.25">
+      <c r="A15" s="31" t="s">
         <v>190</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28">
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27">
         <v>1700</v>
       </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="29">
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="28">
         <v>1703</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="28">
         <v>3</v>
       </c>
-      <c r="K15" s="30" t="s">
+      <c r="K15" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="L15" s="29" t="s">
+      <c r="L15" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="M15" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N15" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O15" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P15" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q15" s="30" t="s">
+      <c r="M15" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O15" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P15" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q15" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="R15" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S15" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T15" s="37" t="s">
+      <c r="R15" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S15" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T15" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="U15" s="38" t="s">
+      <c r="U15" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="V15" s="32" t="s">
+      <c r="V15" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="W15" s="30"/>
-    </row>
-    <row r="16" spans="1:23" s="24" customFormat="1" ht="51.75">
-      <c r="A16" s="32" t="s">
+      <c r="W15" s="29"/>
+    </row>
+    <row r="16" spans="1:23" s="23" customFormat="1" ht="51.75">
+      <c r="A16" s="31" t="s">
         <v>197</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28">
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27">
         <v>1703</v>
       </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="29">
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="28">
         <v>1707</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="28">
         <v>4</v>
       </c>
-      <c r="K16" s="30" t="s">
+      <c r="K16" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L16" s="29" t="s">
+      <c r="L16" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="M16" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N16" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O16" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P16" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q16" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R16" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S16" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T16" s="37" t="s">
+      <c r="M16" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N16" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O16" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P16" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q16" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R16" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S16" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T16" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="U16" s="38" t="s">
+      <c r="U16" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="V16" s="42"/>
-      <c r="W16" s="30"/>
-    </row>
-    <row r="17" spans="1:23" s="24" customFormat="1" ht="38.25">
-      <c r="A17" s="32" t="s">
+      <c r="V16" s="41"/>
+      <c r="W16" s="29"/>
+    </row>
+    <row r="17" spans="1:23" s="23" customFormat="1" ht="38.25">
+      <c r="A17" s="31" t="s">
         <v>202</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28">
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27">
         <v>1707</v>
       </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="29">
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="28">
         <v>1708</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="28">
         <v>0.5</v>
       </c>
-      <c r="K17" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="L17" s="29" t="s">
+      <c r="K17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L17" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="M17" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N17" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O17" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P17" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q17" s="30" t="s">
+      <c r="M17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q17" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="R17" s="30">
+      <c r="R17" s="29">
         <v>1</v>
       </c>
-      <c r="S17" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T17" s="37" t="s">
+      <c r="S17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T17" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="U17" s="38" t="s">
+      <c r="U17" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="V17" s="32" t="s">
+      <c r="V17" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="W17" s="30"/>
-    </row>
-    <row r="18" spans="1:23" s="24" customFormat="1" ht="39">
-      <c r="A18" s="32" t="s">
+      <c r="W17" s="29"/>
+    </row>
+    <row r="18" spans="1:23" s="23" customFormat="1" ht="39">
+      <c r="A18" s="31" t="s">
         <v>208</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28">
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27">
         <v>1708</v>
       </c>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="29">
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="28">
         <v>1708</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="28">
         <v>0.5</v>
       </c>
-      <c r="K18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="L18" s="29" t="s">
+      <c r="K18" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="M18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q18" s="30" t="s">
+      <c r="M18" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O18" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P18" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q18" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="R18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T18" s="37" t="s">
+      <c r="R18" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S18" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T18" s="36" t="s">
         <v>211</v>
       </c>
-      <c r="U18" s="38" t="s">
+      <c r="U18" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="V18" s="42"/>
-      <c r="W18" s="30"/>
-    </row>
-    <row r="19" spans="1:23" s="24" customFormat="1" ht="38.25">
-      <c r="A19" s="32" t="s">
+      <c r="V18" s="41"/>
+      <c r="W18" s="29"/>
+    </row>
+    <row r="19" spans="1:23" s="23" customFormat="1" ht="38.25">
+      <c r="A19" s="31" t="s">
         <v>213</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28">
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27">
         <v>1709</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="29">
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="28">
         <v>1710</v>
       </c>
-      <c r="J19" s="29">
+      <c r="J19" s="28">
         <v>1</v>
       </c>
-      <c r="K19" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="L19" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="M19" s="30">
+      <c r="K19" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="M19" s="29">
         <v>1</v>
       </c>
-      <c r="N19" s="30" t="s">
+      <c r="N19" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="O19" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P19" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q19" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R19" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S19" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T19" s="37" t="s">
+      <c r="O19" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P19" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q19" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R19" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S19" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T19" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="U19" s="38"/>
-      <c r="V19" s="42"/>
-      <c r="W19" s="30"/>
-    </row>
-    <row r="20" spans="1:23" s="24" customFormat="1" ht="51.75">
-      <c r="A20" s="32" t="s">
+      <c r="U19" s="37"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="29"/>
+    </row>
+    <row r="20" spans="1:23" s="23" customFormat="1" ht="51.75">
+      <c r="A20" s="31" t="s">
         <v>218</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28">
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27">
         <v>1710</v>
       </c>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29">
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="28">
         <v>1710</v>
       </c>
-      <c r="J20" s="29">
+      <c r="J20" s="28">
         <f t="shared" ref="J20:J21" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K20" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="L20" s="29" t="s">
+      <c r="K20" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L20" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="M20" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N20" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O20" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P20" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q20" s="30" t="s">
+      <c r="M20" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N20" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O20" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P20" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q20" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="R20" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S20" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T20" s="37" t="s">
+      <c r="R20" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S20" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T20" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="U20" s="38" t="s">
+      <c r="U20" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="V20" s="42"/>
-      <c r="W20" s="30"/>
-    </row>
-    <row r="21" spans="1:23" s="24" customFormat="1" ht="39">
-      <c r="A21" s="32" t="s">
+      <c r="V20" s="41"/>
+      <c r="W20" s="29"/>
+    </row>
+    <row r="21" spans="1:23" s="23" customFormat="1" ht="39">
+      <c r="A21" s="31" t="s">
         <v>222</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28">
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27">
         <v>1710</v>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="29">
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="28">
         <v>1710</v>
       </c>
-      <c r="J21" s="29">
+      <c r="J21" s="28">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K21" s="30" t="s">
+      <c r="K21" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="L21" s="29" t="s">
+      <c r="L21" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M21" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N21" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O21" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P21" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q21" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R21" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S21" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T21" s="37" t="s">
+      <c r="M21" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N21" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O21" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P21" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q21" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R21" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S21" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T21" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="U21" s="38" t="s">
+      <c r="U21" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="V21" s="42"/>
-      <c r="W21" s="30"/>
-    </row>
-    <row r="22" spans="1:23" s="24" customFormat="1" ht="150">
-      <c r="A22" s="32" t="s">
+      <c r="V21" s="41"/>
+      <c r="W21" s="29"/>
+    </row>
+    <row r="22" spans="1:23" s="23" customFormat="1" ht="150">
+      <c r="A22" s="31" t="s">
         <v>227</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28">
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27">
         <v>1710</v>
       </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="29">
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="28">
         <v>1713</v>
       </c>
-      <c r="J22" s="29">
+      <c r="J22" s="28">
         <v>3</v>
       </c>
-      <c r="K22" s="30" t="s">
+      <c r="K22" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="L22" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="M22" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N22" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O22" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P22" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q22" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R22" s="30">
+      <c r="L22" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="M22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R22" s="29">
         <v>1</v>
       </c>
-      <c r="S22" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T22" s="37" t="s">
+      <c r="S22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T22" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="U22" s="38" t="s">
+      <c r="U22" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="V22" s="32" t="s">
+      <c r="V22" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="W22" s="30"/>
-    </row>
-    <row r="23" spans="1:23" s="24" customFormat="1" ht="295.5">
-      <c r="A23" s="32" t="s">
+      <c r="W22" s="29"/>
+    </row>
+    <row r="23" spans="1:23" s="23" customFormat="1" ht="295.5">
+      <c r="A23" s="31" t="s">
         <v>233</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28">
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27">
         <v>1713</v>
       </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="29">
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="28">
         <v>1736</v>
       </c>
-      <c r="J23" s="29">
+      <c r="J23" s="28">
         <v>23</v>
       </c>
-      <c r="K23" s="30" t="s">
+      <c r="K23" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="L23" s="29" t="s">
+      <c r="L23" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M23" s="30">
+      <c r="M23" s="29">
         <v>1</v>
       </c>
-      <c r="N23" s="30" t="s">
+      <c r="N23" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="O23" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P23" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q23" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R23" s="30">
+      <c r="O23" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P23" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q23" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R23" s="29">
         <v>1</v>
       </c>
-      <c r="S23" s="30" t="s">
+      <c r="S23" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="T23" s="37" t="s">
+      <c r="T23" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="U23" s="38" t="s">
+      <c r="U23" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="V23" s="43" t="s">
+      <c r="V23" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="W23" s="30"/>
-    </row>
-    <row r="24" spans="1:23" s="24" customFormat="1" ht="102.75">
-      <c r="A24" s="32" t="s">
+      <c r="W23" s="29"/>
+    </row>
+    <row r="24" spans="1:23" s="23" customFormat="1" ht="102.75">
+      <c r="A24" s="31" t="s">
         <v>240</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28">
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27">
         <v>1736</v>
       </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="29">
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="28">
         <v>1754</v>
       </c>
-      <c r="J24" s="29">
+      <c r="J24" s="28">
         <v>18</v>
       </c>
-      <c r="K24" s="30" t="s">
+      <c r="K24" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="L24" s="29" t="s">
+      <c r="L24" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M24" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N24" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O24" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P24" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q24" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R24" s="30">
+      <c r="M24" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N24" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O24" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P24" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q24" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R24" s="29">
         <v>1</v>
       </c>
-      <c r="S24" s="30" t="s">
+      <c r="S24" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="T24" s="37" t="s">
+      <c r="T24" s="36" t="s">
         <v>243</v>
       </c>
-      <c r="U24" s="38" t="s">
+      <c r="U24" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="V24" s="30" t="s">
+      <c r="V24" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="W24" s="30"/>
-    </row>
-    <row r="25" spans="1:23" s="24" customFormat="1" ht="77.25">
-      <c r="A25" s="32" t="s">
+      <c r="W24" s="29"/>
+    </row>
+    <row r="25" spans="1:23" s="23" customFormat="1" ht="77.25">
+      <c r="A25" s="31" t="s">
         <v>246</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28">
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27">
         <v>1754</v>
       </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="29">
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="28">
         <v>1756</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25" s="28">
         <v>2</v>
       </c>
-      <c r="K25" s="30" t="s">
+      <c r="K25" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="L25" s="29" t="s">
+      <c r="L25" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M25" s="30">
+      <c r="M25" s="29">
         <v>1</v>
       </c>
-      <c r="N25" s="30" t="s">
+      <c r="N25" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="O25" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P25" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q25" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R25" s="30">
+      <c r="O25" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P25" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q25" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R25" s="29">
         <v>1</v>
       </c>
-      <c r="S25" s="30" t="s">
+      <c r="S25" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="T25" s="37" t="s">
+      <c r="T25" s="36" t="s">
         <v>249</v>
       </c>
-      <c r="U25" s="38" t="s">
+      <c r="U25" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="V25" s="30" t="s">
+      <c r="V25" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="W25" s="30"/>
-    </row>
-    <row r="26" spans="1:23" s="24" customFormat="1" ht="102.75">
-      <c r="A26" s="32" t="s">
+      <c r="W25" s="29"/>
+    </row>
+    <row r="26" spans="1:23" s="23" customFormat="1" ht="102.75">
+      <c r="A26" s="31" t="s">
         <v>252</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28">
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27">
         <v>1756</v>
       </c>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="29">
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="28">
         <v>1771</v>
       </c>
-      <c r="J26" s="29">
+      <c r="J26" s="28">
         <v>15</v>
       </c>
-      <c r="K26" s="30" t="s">
+      <c r="K26" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="L26" s="29" t="s">
+      <c r="L26" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M26" s="30">
+      <c r="M26" s="29">
         <v>1</v>
       </c>
-      <c r="N26" s="30" t="s">
+      <c r="N26" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="O26" s="30" t="s">
+      <c r="O26" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="P26" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q26" s="30" t="s">
+      <c r="P26" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q26" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="R26" s="30">
+      <c r="R26" s="29">
         <v>2</v>
       </c>
-      <c r="S26" s="30" t="s">
+      <c r="S26" s="29" t="s">
         <v>257</v>
       </c>
-      <c r="T26" s="37" t="s">
+      <c r="T26" s="36" t="s">
         <v>258</v>
       </c>
-      <c r="U26" s="38" t="s">
+      <c r="U26" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="V26" s="30" t="s">
+      <c r="V26" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="W26" s="30"/>
-    </row>
-    <row r="27" spans="1:23" s="24" customFormat="1" ht="153.75">
-      <c r="A27" s="16" t="s">
+      <c r="W26" s="29"/>
+    </row>
+    <row r="27" spans="1:23" s="23" customFormat="1" ht="153.75">
+      <c r="A27" s="50" t="s">
         <v>261</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="35" t="s">
         <v>263</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28">
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27">
         <v>1771</v>
       </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="29">
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="28">
         <v>1792</v>
       </c>
-      <c r="J27" s="29">
+      <c r="J27" s="28">
         <v>21</v>
       </c>
-      <c r="K27" s="30" t="s">
+      <c r="K27" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L27" s="29" t="s">
+      <c r="L27" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M27" s="30">
+      <c r="M27" s="29">
         <v>1</v>
       </c>
-      <c r="N27" s="30" t="s">
+      <c r="N27" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="O27" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P27" s="30" t="s">
+      <c r="O27" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P27" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="Q27" s="30" t="s">
+      <c r="Q27" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="R27" s="30">
+      <c r="R27" s="29">
         <v>2</v>
       </c>
-      <c r="S27" s="30" t="s">
+      <c r="S27" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="T27" s="31" t="s">
+      <c r="T27" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="U27" s="38" t="s">
+      <c r="U27" s="37" t="s">
         <v>267</v>
       </c>
-      <c r="V27" s="30" t="s">
+      <c r="V27" s="29" t="s">
         <v>268</v>
       </c>
-      <c r="W27" s="30"/>
-    </row>
-    <row r="28" spans="1:23" s="24" customFormat="1" ht="85.5">
-      <c r="A28" s="44" t="s">
+      <c r="W27" s="29"/>
+    </row>
+    <row r="28" spans="1:23" s="23" customFormat="1" ht="85.5">
+      <c r="A28" s="43" t="s">
         <v>269</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="44" t="s">
         <v>270</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28">
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27">
         <v>1792</v>
       </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="29">
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="28">
         <v>1792</v>
       </c>
-      <c r="J28" s="29">
+      <c r="J28" s="28">
         <f>3/365</f>
         <v>8.21917808219178E-3</v>
       </c>
-      <c r="K28" s="30" t="s">
+      <c r="K28" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L28" s="29" t="s">
+      <c r="L28" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M28" s="30">
+      <c r="M28" s="29">
         <v>1</v>
       </c>
-      <c r="N28" s="30" t="s">
+      <c r="N28" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="O28" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P28" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q28" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R28" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S28" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T28" s="37" t="s">
+      <c r="O28" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P28" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q28" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R28" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S28" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T28" s="36" t="s">
         <v>272</v>
       </c>
-      <c r="U28" s="38" t="s">
+      <c r="U28" s="37" t="s">
         <v>273</v>
       </c>
-      <c r="V28" s="42"/>
-      <c r="W28" s="30"/>
-    </row>
-    <row r="29" spans="1:23" s="24" customFormat="1" ht="127.5">
-      <c r="A29" s="32" t="s">
+      <c r="V28" s="41"/>
+      <c r="W28" s="29"/>
+    </row>
+    <row r="29" spans="1:23" s="23" customFormat="1" ht="127.5">
+      <c r="A29" s="31" t="s">
         <v>274</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="35" t="s">
         <v>276</v>
       </c>
-      <c r="D29" s="28">
+      <c r="D29" s="27">
         <v>9</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29" s="27">
         <v>1</v>
       </c>
-      <c r="F29" s="28">
+      <c r="F29" s="27">
         <v>1792</v>
       </c>
-      <c r="G29" s="28">
+      <c r="G29" s="27">
         <v>1</v>
       </c>
-      <c r="H29" s="28">
+      <c r="H29" s="27">
         <v>30</v>
       </c>
-      <c r="I29" s="29">
+      <c r="I29" s="28">
         <v>1795</v>
       </c>
-      <c r="J29" s="29">
+      <c r="J29" s="28">
         <v>3</v>
       </c>
-      <c r="K29" s="30" t="s">
+      <c r="K29" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L29" s="29" t="s">
+      <c r="L29" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="M29" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="N29" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="O29" s="30" t="s">
+      <c r="M29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O29" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="P29" s="30" t="s">
+      <c r="P29" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="Q29" s="30" t="s">
+      <c r="Q29" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="R29" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S29" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T29" s="37" t="s">
+      <c r="R29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T29" s="36" t="s">
         <v>277</v>
       </c>
-      <c r="U29" s="38" t="s">
+      <c r="U29" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="V29" s="32" t="s">
+      <c r="V29" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="W29" s="30" t="s">
+      <c r="W29" s="29" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="24" customFormat="1" ht="115.5">
-      <c r="A30" s="32" t="s">
+    <row r="30" spans="1:23" s="23" customFormat="1" ht="115.5">
+      <c r="A30" s="31" t="s">
         <v>281</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>283</v>
       </c>
-      <c r="D30" s="28">
+      <c r="D30" s="27">
         <v>2</v>
       </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28">
+      <c r="E30" s="27"/>
+      <c r="F30" s="27">
         <v>1795</v>
       </c>
-      <c r="G30" s="28">
+      <c r="G30" s="27">
         <v>1</v>
       </c>
-      <c r="H30" s="28"/>
-      <c r="I30" s="29">
+      <c r="H30" s="27"/>
+      <c r="I30" s="28">
         <v>1798</v>
       </c>
-      <c r="J30" s="29">
+      <c r="J30" s="28">
         <v>3</v>
       </c>
-      <c r="K30" s="30" t="s">
+      <c r="K30" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L30" s="29" t="s">
+      <c r="L30" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M30" s="30">
+      <c r="M30" s="29">
         <v>1</v>
       </c>
-      <c r="N30" s="30" t="s">
+      <c r="N30" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="O30" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P30" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q30" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R30" s="30">
+      <c r="O30" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P30" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q30" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R30" s="29">
         <v>1</v>
       </c>
-      <c r="S30" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T30" s="37" t="s">
+      <c r="S30" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T30" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="U30" s="38" t="s">
+      <c r="U30" s="37" t="s">
         <v>285</v>
       </c>
-      <c r="V30" s="32" t="s">
+      <c r="V30" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="W30" s="30" t="s">
+      <c r="W30" s="29" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="31" spans="1:23" s="24" customFormat="1" ht="191.25">
-      <c r="A31" s="32" t="s">
+    <row r="31" spans="1:23" s="23" customFormat="1" ht="191.25">
+      <c r="A31" s="31" t="s">
         <v>288</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="27">
         <v>1</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28">
+      <c r="E31" s="27"/>
+      <c r="F31" s="27">
         <v>1798</v>
       </c>
-      <c r="G31" s="28">
+      <c r="G31" s="27">
         <v>5</v>
       </c>
-      <c r="H31" s="28"/>
-      <c r="I31" s="29">
+      <c r="H31" s="27"/>
+      <c r="I31" s="28">
         <v>1803</v>
       </c>
-      <c r="J31" s="29">
+      <c r="J31" s="28">
         <v>5</v>
       </c>
-      <c r="K31" s="30" t="s">
+      <c r="K31" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="L31" s="29" t="s">
+      <c r="L31" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M31" s="30">
+      <c r="M31" s="29">
         <v>1</v>
       </c>
-      <c r="N31" s="30" t="s">
+      <c r="N31" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="O31" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P31" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q31" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R31" s="30">
+      <c r="O31" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P31" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q31" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R31" s="29">
         <v>1</v>
       </c>
-      <c r="S31" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T31" s="37" t="s">
+      <c r="S31" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T31" s="36" t="s">
         <v>291</v>
       </c>
-      <c r="U31" s="38" t="s">
+      <c r="U31" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="V31" s="32" t="s">
+      <c r="V31" s="31" t="s">
         <v>293</v>
       </c>
-      <c r="W31" s="30" t="s">
+      <c r="W31" s="29" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="32" spans="1:23" s="24" customFormat="1" ht="115.5">
-      <c r="A32" s="32" t="s">
+    <row r="32" spans="1:23" s="23" customFormat="1" ht="115.5">
+      <c r="A32" s="31" t="s">
         <v>295</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="D32" s="28">
+      <c r="D32" s="27">
         <v>5</v>
       </c>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28">
+      <c r="E32" s="27"/>
+      <c r="F32" s="27">
         <v>1803</v>
       </c>
-      <c r="G32" s="28">
+      <c r="G32" s="27">
         <v>11</v>
       </c>
-      <c r="H32" s="28"/>
-      <c r="I32" s="29">
+      <c r="H32" s="27"/>
+      <c r="I32" s="28">
         <v>1804</v>
       </c>
-      <c r="J32" s="29">
+      <c r="J32" s="28">
         <v>1</v>
       </c>
-      <c r="K32" s="30" t="s">
+      <c r="K32" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="L32" s="29" t="s">
+      <c r="L32" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="M32" s="30">
+      <c r="M32" s="29">
         <v>1</v>
       </c>
-      <c r="N32" s="30" t="s">
+      <c r="N32" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="O32" s="30" t="s">
+      <c r="O32" s="29" t="s">
         <v>298</v>
       </c>
-      <c r="P32" s="30" t="s">
+      <c r="P32" s="29" t="s">
         <v>298</v>
       </c>
-      <c r="Q32" s="30" t="s">
+      <c r="Q32" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="R32" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S32" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T32" s="37" t="s">
+      <c r="R32" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S32" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T32" s="36" t="s">
         <v>299</v>
       </c>
-      <c r="U32" s="38" t="s">
+      <c r="U32" s="37" t="s">
         <v>300</v>
       </c>
-      <c r="V32" s="42"/>
-      <c r="W32" s="30" t="s">
+      <c r="V32" s="41"/>
+      <c r="W32" s="29" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="24" customFormat="1" ht="165.75">
-      <c r="A33" s="32" t="s">
+    <row r="33" spans="1:23" s="23" customFormat="1" ht="165.75">
+      <c r="A33" s="31" t="s">
         <v>302</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="27">
         <v>11</v>
       </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28">
+      <c r="E33" s="27"/>
+      <c r="F33" s="27">
         <v>1804</v>
       </c>
-      <c r="G33" s="28">
+      <c r="G33" s="27">
         <v>12</v>
       </c>
-      <c r="H33" s="28"/>
-      <c r="I33" s="29">
+      <c r="H33" s="27"/>
+      <c r="I33" s="28">
         <v>1806</v>
       </c>
-      <c r="J33" s="29">
+      <c r="J33" s="28">
         <v>2</v>
       </c>
-      <c r="K33" s="30" t="s">
+      <c r="K33" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L33" s="29" t="s">
+      <c r="L33" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M33" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="N33" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="O33" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="P33" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q33" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="R33" s="30">
+      <c r="M33" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="N33" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="O33" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="P33" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q33" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="R33" s="29">
         <v>1</v>
       </c>
-      <c r="S33" s="46" t="s">
+      <c r="S33" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="T33" s="37" t="s">
+      <c r="T33" s="36" t="s">
         <v>305</v>
       </c>
-      <c r="U33" s="39" t="s">
+      <c r="U33" s="38" t="s">
         <v>306</v>
       </c>
-      <c r="V33" s="32" t="s">
+      <c r="V33" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="W33" s="31" t="s">
+      <c r="W33" s="30" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="24" customFormat="1" ht="102">
-      <c r="A34" s="32" t="s">
+    <row r="34" spans="1:23" s="23" customFormat="1" ht="102">
+      <c r="A34" s="31" t="s">
         <v>309</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="D34" s="28">
+      <c r="D34" s="27">
         <v>12</v>
       </c>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28">
+      <c r="E34" s="27"/>
+      <c r="F34" s="27">
         <v>1806</v>
       </c>
-      <c r="G34" s="28">
+      <c r="G34" s="27">
         <v>7</v>
       </c>
-      <c r="H34" s="28"/>
-      <c r="I34" s="29">
+      <c r="H34" s="27"/>
+      <c r="I34" s="28">
         <v>1807</v>
       </c>
-      <c r="J34" s="29">
+      <c r="J34" s="28">
         <v>1</v>
       </c>
-      <c r="K34" s="30" t="s">
+      <c r="K34" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L34" s="29" t="s">
+      <c r="L34" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="M34" s="30">
+      <c r="M34" s="29">
         <v>0</v>
       </c>
-      <c r="N34" s="30" t="s">
+      <c r="N34" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="O34" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P34" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q34" s="30" t="s">
+      <c r="O34" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P34" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q34" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="R34" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S34" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T34" s="37" t="s">
+      <c r="R34" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S34" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T34" s="36" t="s">
         <v>312</v>
       </c>
-      <c r="U34" s="31" t="s">
+      <c r="U34" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="V34" s="32" t="s">
+      <c r="V34" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="W34" s="30" t="s">
+      <c r="W34" s="29" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="24" customFormat="1" ht="114.75">
-      <c r="A35" s="32" t="s">
+    <row r="35" spans="1:23" s="23" customFormat="1" ht="114.75">
+      <c r="A35" s="31" t="s">
         <v>316</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="35" t="s">
         <v>318</v>
       </c>
-      <c r="D35" s="28">
+      <c r="D35" s="27">
         <v>8</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28">
+      <c r="E35" s="27"/>
+      <c r="F35" s="27">
         <v>1807</v>
       </c>
-      <c r="G35" s="28">
+      <c r="G35" s="27">
         <v>9</v>
       </c>
-      <c r="H35" s="28"/>
-      <c r="I35" s="29">
+      <c r="H35" s="27"/>
+      <c r="I35" s="28">
         <v>1808</v>
       </c>
-      <c r="J35" s="29">
+      <c r="J35" s="28">
         <v>1</v>
       </c>
-      <c r="K35" s="30" t="s">
+      <c r="K35" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L35" s="29" t="s">
+      <c r="L35" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M35" s="30">
+      <c r="M35" s="29">
         <v>1</v>
       </c>
-      <c r="N35" s="30" t="s">
+      <c r="N35" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="O35" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P35" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q35" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R35" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S35" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T35" s="37" t="s">
+      <c r="O35" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P35" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q35" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R35" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S35" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T35" s="36" t="s">
         <v>319</v>
       </c>
-      <c r="U35" s="31" t="s">
+      <c r="U35" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="V35" s="32" t="s">
+      <c r="V35" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="W35" s="30" t="s">
+      <c r="W35" s="29" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="36" spans="1:23" s="24" customFormat="1" ht="89.25">
-      <c r="A36" s="32" t="s">
+    <row r="36" spans="1:23" s="23" customFormat="1" ht="89.25">
+      <c r="A36" s="31" t="s">
         <v>323</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="D36" s="28">
+      <c r="D36" s="27">
         <v>9</v>
       </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28">
+      <c r="E36" s="27"/>
+      <c r="F36" s="27">
         <v>1808</v>
       </c>
-      <c r="G36" s="28">
+      <c r="G36" s="27">
         <v>9</v>
       </c>
-      <c r="H36" s="28"/>
-      <c r="I36" s="29">
+      <c r="H36" s="27"/>
+      <c r="I36" s="28">
         <v>1808</v>
       </c>
-      <c r="J36" s="29">
+      <c r="J36" s="28">
         <f>15/365</f>
         <v>4.1095890410958902E-2</v>
       </c>
-      <c r="K36" s="30" t="s">
+      <c r="K36" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L36" s="29" t="s">
+      <c r="L36" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M36" s="30">
+      <c r="M36" s="29">
         <v>1</v>
       </c>
-      <c r="N36" s="30" t="s">
+      <c r="N36" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="O36" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P36" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q36" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R36" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S36" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T36" s="37" t="s">
+      <c r="O36" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P36" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q36" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R36" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S36" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T36" s="36" t="s">
         <v>326</v>
       </c>
-      <c r="U36" s="31" t="s">
+      <c r="U36" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="V36" s="32" t="s">
+      <c r="V36" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="W36" s="30" t="s">
+      <c r="W36" s="29" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="37" spans="1:23" s="24" customFormat="1" ht="255">
-      <c r="A37" s="32" t="s">
+    <row r="37" spans="1:23" s="23" customFormat="1" ht="255">
+      <c r="A37" s="31" t="s">
         <v>330</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="35" t="s">
         <v>332</v>
       </c>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28">
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27">
         <v>1808</v>
       </c>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="29">
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="28">
         <v>1811</v>
       </c>
-      <c r="J37" s="29">
+      <c r="J37" s="28">
         <v>3</v>
       </c>
-      <c r="K37" s="30" t="s">
+      <c r="K37" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L37" s="29" t="s">
+      <c r="L37" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M37" s="30">
+      <c r="M37" s="29">
         <v>1</v>
       </c>
-      <c r="N37" s="30" t="s">
+      <c r="N37" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="O37" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P37" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q37" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R37" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S37" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T37" s="37" t="s">
+      <c r="O37" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P37" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q37" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R37" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S37" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T37" s="36" t="s">
         <v>333</v>
       </c>
-      <c r="U37" s="31" t="s">
+      <c r="U37" s="30" t="s">
         <v>334</v>
       </c>
-      <c r="V37" s="32" t="s">
+      <c r="V37" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="W37" s="47" t="s">
+      <c r="W37" s="46" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="38" spans="1:23" s="24" customFormat="1" ht="255">
-      <c r="A38" s="32" t="s">
+    <row r="38" spans="1:23" s="23" customFormat="1" ht="255">
+      <c r="A38" s="31" t="s">
         <v>337</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>338</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28">
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27">
         <v>1811</v>
       </c>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="29">
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="28">
         <v>1814</v>
       </c>
-      <c r="J38" s="29">
+      <c r="J38" s="28">
         <v>3</v>
       </c>
-      <c r="K38" s="30" t="s">
+      <c r="K38" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L38" s="29" t="s">
+      <c r="L38" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M38" s="30">
+      <c r="M38" s="29">
         <v>1</v>
       </c>
-      <c r="N38" s="30" t="s">
+      <c r="N38" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="O38" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P38" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q38" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R38" s="30">
+      <c r="O38" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P38" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q38" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R38" s="29">
         <v>1</v>
       </c>
-      <c r="S38" s="30" t="s">
+      <c r="S38" s="29" t="s">
         <v>340</v>
       </c>
-      <c r="T38" s="37" t="s">
+      <c r="T38" s="36" t="s">
         <v>341</v>
       </c>
-      <c r="U38" s="32" t="s">
+      <c r="U38" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="V38" s="32" t="s">
+      <c r="V38" s="31" t="s">
         <v>343</v>
       </c>
-      <c r="W38" s="30"/>
-    </row>
-    <row r="39" spans="1:23" s="24" customFormat="1" ht="177">
-      <c r="A39" s="32" t="s">
+      <c r="W38" s="29"/>
+    </row>
+    <row r="39" spans="1:23" s="23" customFormat="1" ht="177">
+      <c r="A39" s="31" t="s">
         <v>344</v>
       </c>
       <c r="B39" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="35" t="s">
         <v>346</v>
       </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28">
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27">
         <v>1814</v>
       </c>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="29">
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="28">
         <v>1818</v>
       </c>
-      <c r="J39" s="29">
+      <c r="J39" s="28">
         <v>4</v>
       </c>
-      <c r="K39" s="30" t="s">
+      <c r="K39" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L39" s="29" t="s">
+      <c r="L39" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M39" s="30">
+      <c r="M39" s="29">
         <v>1</v>
       </c>
-      <c r="N39" s="30" t="s">
+      <c r="N39" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="O39" s="30" t="s">
+      <c r="O39" s="29" t="s">
         <v>347</v>
       </c>
-      <c r="P39" s="30" t="s">
+      <c r="P39" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="Q39" s="30" t="s">
+      <c r="Q39" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="R39" s="30">
+      <c r="R39" s="29">
         <v>1</v>
       </c>
-      <c r="S39" s="30" t="s">
+      <c r="S39" s="29" t="s">
         <v>348</v>
       </c>
-      <c r="T39" s="37" t="s">
+      <c r="T39" s="36" t="s">
         <v>349</v>
       </c>
-      <c r="U39" s="38" t="s">
+      <c r="U39" s="37" t="s">
         <v>350</v>
       </c>
-      <c r="V39" s="32" t="s">
+      <c r="V39" s="31" t="s">
         <v>351</v>
       </c>
-      <c r="W39" s="30" t="s">
+      <c r="W39" s="29" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="40" spans="1:23" s="24" customFormat="1" ht="156">
-      <c r="A40" s="32" t="s">
+    <row r="40" spans="1:23" s="23" customFormat="1" ht="156">
+      <c r="A40" s="31" t="s">
         <v>353</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="26" t="s">
         <v>355</v>
       </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28">
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27">
         <v>1818</v>
       </c>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="29">
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="28">
         <v>1818</v>
       </c>
-      <c r="J40" s="29">
+      <c r="J40" s="28">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="K40" s="30" t="s">
+      <c r="K40" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L40" s="29" t="s">
+      <c r="L40" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M40" s="30">
+      <c r="M40" s="29">
         <v>1</v>
       </c>
-      <c r="N40" s="30" t="s">
+      <c r="N40" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="O40" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P40" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q40" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R40" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S40" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T40" s="37" t="s">
+      <c r="O40" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P40" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q40" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R40" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S40" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T40" s="36" t="s">
         <v>356</v>
       </c>
-      <c r="U40" s="38" t="s">
+      <c r="U40" s="37" t="s">
         <v>357</v>
       </c>
-      <c r="V40" s="42"/>
-      <c r="W40" s="30"/>
-    </row>
-    <row r="41" spans="1:23" s="24" customFormat="1" ht="117.75">
-      <c r="A41" s="32" t="s">
+      <c r="V40" s="41"/>
+      <c r="W40" s="29"/>
+    </row>
+    <row r="41" spans="1:23" s="23" customFormat="1" ht="117.75">
+      <c r="A41" s="31" t="s">
         <v>358</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="35" t="s">
         <v>360</v>
       </c>
-      <c r="D41" s="28">
+      <c r="D41" s="27">
         <v>1</v>
       </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28">
+      <c r="E41" s="27"/>
+      <c r="F41" s="27">
         <v>1818</v>
       </c>
-      <c r="G41" s="28">
+      <c r="G41" s="27">
         <v>7</v>
       </c>
-      <c r="H41" s="28"/>
-      <c r="I41" s="29">
+      <c r="H41" s="27"/>
+      <c r="I41" s="28">
         <v>1818</v>
       </c>
-      <c r="J41" s="29">
+      <c r="J41" s="28">
         <v>0.5</v>
       </c>
-      <c r="K41" s="30" t="s">
+      <c r="K41" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="L41" s="29" t="s">
+      <c r="L41" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="M41" s="30">
+      <c r="M41" s="29">
         <v>1</v>
       </c>
-      <c r="N41" s="30" t="s">
+      <c r="N41" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="O41" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P41" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q41" s="30" t="s">
+      <c r="O41" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P41" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q41" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="R41" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S41" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T41" s="37" t="s">
+      <c r="R41" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S41" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T41" s="36" t="s">
         <v>362</v>
       </c>
-      <c r="U41" s="38" t="s">
+      <c r="U41" s="37" t="s">
         <v>363</v>
       </c>
-      <c r="V41" s="32" t="s">
+      <c r="V41" s="31" t="s">
         <v>364</v>
       </c>
-      <c r="W41" s="30" t="s">
+      <c r="W41" s="29" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="42" spans="1:23" s="24" customFormat="1" ht="63.75">
-      <c r="A42" s="32" t="s">
+    <row r="42" spans="1:23" s="23" customFormat="1" ht="63.75">
+      <c r="A42" s="31" t="s">
         <v>366</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>367</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28">
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27">
         <v>1818</v>
       </c>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="29">
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="28">
         <v>1819</v>
       </c>
-      <c r="J42" s="29">
+      <c r="J42" s="28">
         <v>1</v>
       </c>
-      <c r="K42" s="30" t="s">
+      <c r="K42" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M42" s="30">
+      <c r="M42" s="29">
         <v>1</v>
       </c>
-      <c r="N42" s="30" t="s">
+      <c r="N42" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="O42" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P42" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q42" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R42" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S42" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T42" s="37" t="s">
+      <c r="O42" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P42" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q42" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R42" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S42" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T42" s="36" t="s">
         <v>369</v>
       </c>
-      <c r="U42" s="31" t="s">
+      <c r="U42" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="V42" s="32" t="s">
+      <c r="V42" s="31" t="s">
         <v>371</v>
       </c>
-      <c r="W42" s="30"/>
-    </row>
-    <row r="43" spans="1:23" s="24" customFormat="1" ht="204">
-      <c r="A43" s="32" t="s">
+      <c r="W42" s="29"/>
+    </row>
+    <row r="43" spans="1:23" s="23" customFormat="1" ht="204">
+      <c r="A43" s="31" t="s">
         <v>372</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="35" t="s">
         <v>374</v>
       </c>
-      <c r="D43" s="28">
+      <c r="D43" s="27">
         <v>6</v>
       </c>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28">
+      <c r="E43" s="27"/>
+      <c r="F43" s="27">
         <v>1819</v>
       </c>
-      <c r="G43" s="28">
+      <c r="G43" s="27">
         <v>7</v>
       </c>
-      <c r="H43" s="28"/>
-      <c r="I43" s="29">
+      <c r="H43" s="27"/>
+      <c r="I43" s="28">
         <v>1820</v>
       </c>
-      <c r="J43" s="29">
+      <c r="J43" s="28">
         <v>1</v>
       </c>
-      <c r="K43" s="30" t="s">
+      <c r="K43" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L43" s="29" t="s">
+      <c r="L43" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M43" s="30">
+      <c r="M43" s="29">
         <v>1</v>
       </c>
-      <c r="N43" s="30" t="s">
+      <c r="N43" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="O43" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P43" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q43" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="R43" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S43" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T43" s="37" t="s">
+      <c r="O43" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P43" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q43" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R43" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S43" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T43" s="36" t="s">
         <v>375</v>
       </c>
-      <c r="U43" s="31" t="s">
+      <c r="U43" s="30" t="s">
         <v>376</v>
       </c>
-      <c r="V43" s="32" t="s">
+      <c r="V43" s="31" t="s">
         <v>377</v>
       </c>
-      <c r="W43" s="30" t="s">
+      <c r="W43" s="29" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="44" spans="1:23" s="24" customFormat="1" ht="57.75">
-      <c r="A44" s="32" t="s">
+    <row r="44" spans="1:23" s="23" customFormat="1" ht="57.75">
+      <c r="A44" s="31" t="s">
         <v>358</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="25" t="s">
         <v>359</v>
       </c>
-      <c r="C44" s="27" t="s">
+      <c r="C44" s="26" t="s">
         <v>360</v>
       </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28">
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27">
         <v>1820</v>
       </c>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="29">
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="28">
         <v>1822</v>
       </c>
-      <c r="J44" s="29">
+      <c r="J44" s="28">
         <v>2</v>
       </c>
-      <c r="K44" s="30" t="s">
+      <c r="K44" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="L44" s="29" t="s">
+      <c r="L44" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="M44" s="30">
+      <c r="M44" s="29">
         <v>1</v>
       </c>
-      <c r="N44" s="30" t="s">
+      <c r="N44" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="O44" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P44" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q44" s="30" t="s">
+      <c r="O44" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P44" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q44" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="R44" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S44" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T44" s="37" t="s">
+      <c r="R44" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S44" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T44" s="36" t="s">
         <v>379</v>
       </c>
-      <c r="U44" s="38" t="s">
+      <c r="U44" s="37" t="s">
         <v>380</v>
       </c>
-      <c r="V44" s="42"/>
-      <c r="W44" s="30"/>
-    </row>
-    <row r="45" spans="1:23" s="24" customFormat="1" ht="132.75">
-      <c r="A45" s="32" t="s">
+      <c r="V44" s="41"/>
+      <c r="W44" s="29"/>
+    </row>
+    <row r="45" spans="1:23" s="23" customFormat="1" ht="132.75">
+      <c r="A45" s="31" t="s">
         <v>381</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="C45" s="36" t="s">
+      <c r="C45" s="35" t="s">
         <v>383</v>
       </c>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28">
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27">
         <v>1822</v>
       </c>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="29">
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="28">
         <v>1824</v>
       </c>
-      <c r="J45" s="29">
+      <c r="J45" s="28">
         <v>2</v>
       </c>
-      <c r="K45" s="30" t="s">
+      <c r="K45" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="L45" s="29" t="s">
+      <c r="L45" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M45" s="30">
+      <c r="M45" s="29">
         <v>1</v>
       </c>
-      <c r="N45" s="30" t="s">
+      <c r="N45" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="O45" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P45" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q45" s="30" t="s">
+      <c r="O45" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P45" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q45" s="29" t="s">
         <v>384</v>
       </c>
-      <c r="R45" s="30">
+      <c r="R45" s="29">
         <v>1</v>
       </c>
-      <c r="S45" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T45" s="37" t="s">
+      <c r="S45" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T45" s="36" t="s">
         <v>385</v>
       </c>
-      <c r="U45" s="38" t="s">
+      <c r="U45" s="37" t="s">
         <v>386</v>
       </c>
-      <c r="V45" s="32" t="s">
+      <c r="V45" s="31" t="s">
         <v>387</v>
       </c>
-      <c r="W45" s="30"/>
-    </row>
-    <row r="46" spans="1:23" s="24" customFormat="1" ht="51">
-      <c r="A46" s="32" t="s">
+      <c r="W45" s="29"/>
+    </row>
+    <row r="46" spans="1:23" s="23" customFormat="1" ht="51">
+      <c r="A46" s="31" t="s">
         <v>388</v>
       </c>
       <c r="B46" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="C46" s="26" t="s">
         <v>390</v>
       </c>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28">
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27">
         <v>1824</v>
       </c>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="29">
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="28">
         <v>1826</v>
       </c>
-      <c r="J46" s="29">
+      <c r="J46" s="28">
         <v>2</v>
       </c>
-      <c r="K46" s="30" t="s">
+      <c r="K46" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="L46" s="29" t="s">
+      <c r="L46" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="M46" s="30">
+      <c r="M46" s="29">
         <v>1</v>
       </c>
-      <c r="N46" s="30" t="s">
+      <c r="N46" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="O46" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P46" s="30" t="s">
+      <c r="O46" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P46" s="29" t="s">
         <v>391</v>
       </c>
-      <c r="Q46" s="30" t="s">
+      <c r="Q46" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="R46" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="S46" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T46" s="37" t="s">
+      <c r="R46" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S46" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T46" s="36" t="s">
         <v>392</v>
       </c>
-      <c r="U46" s="38" t="s">
+      <c r="U46" s="37" t="s">
         <v>393</v>
       </c>
-      <c r="V46" s="42"/>
-      <c r="W46" s="30"/>
-    </row>
-    <row r="47" spans="1:23" s="24" customFormat="1" ht="106.5">
-      <c r="A47" s="32" t="s">
+      <c r="V46" s="41"/>
+      <c r="W46" s="29"/>
+    </row>
+    <row r="47" spans="1:23" s="23" customFormat="1" ht="106.5">
+      <c r="A47" s="31" t="s">
         <v>394</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>395</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C47" s="35" t="s">
         <v>396</v>
       </c>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28">
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27">
         <v>1826</v>
       </c>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="29">
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="28">
         <v>1837</v>
       </c>
-      <c r="J47" s="29">
+      <c r="J47" s="28">
         <v>11</v>
       </c>
-      <c r="K47" s="48" t="s">
+      <c r="K47" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="L47" s="29" t="s">
+      <c r="L47" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="M47" s="30">
+      <c r="M47" s="29">
         <v>1</v>
       </c>
-      <c r="N47" s="30" t="s">
+      <c r="N47" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="O47" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="P47" s="30" t="s">
+      <c r="O47" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="P47" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="Q47" s="30" t="s">
+      <c r="Q47" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="R47" s="30">
+      <c r="R47" s="29">
         <v>7</v>
       </c>
-      <c r="S47" s="30" t="s">
+      <c r="S47" s="29" t="s">
         <v>397</v>
       </c>
-      <c r="T47" s="37" t="s">
+      <c r="T47" s="36" t="s">
         <v>398</v>
       </c>
-      <c r="U47" s="38" t="s">
+      <c r="U47" s="37" t="s">
         <v>399</v>
       </c>
-      <c r="V47" s="42"/>
-      <c r="W47" s="30"/>
+      <c r="V47" s="41"/>
+      <c r="W47" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -5189,8 +5182,8 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5246,8 +5239,8 @@
       <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>403</v>
+      <c r="C2" s="49" t="s">
+        <v>402</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>23</v>
@@ -5311,7 +5304,7 @@
       <c r="Y3" s="10"/>
       <c r="Z3" s="10"/>
     </row>
-    <row r="4" spans="1:26" ht="180">
+    <row r="4" spans="1:26" ht="165">
       <c r="A4" s="6" t="s">
         <v>33</v>
       </c>
@@ -5324,8 +5317,8 @@
       <c r="D4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="51" t="s">
-        <v>401</v>
+      <c r="E4" s="48" t="s">
+        <v>403</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -5460,8 +5453,8 @@
       <c r="B8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="51" t="s">
-        <v>402</v>
+      <c r="C8" s="48" t="s">
+        <v>401</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>67</v>
@@ -10676,7 +10669,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -10690,14 +10683,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="3" t="s">
@@ -11145,14 +11138,14 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">

</xml_diff>